<commit_message>
added last proc date
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/MDOT/Scenarios/MDOT/TS_SM_FOU_PcaGroupProfile_Regression_001.xlsx
+++ b/src/main/java/TestSuite/MDOT/Scenarios/MDOT/TS_SM_FOU_PcaGroupProfile_Regression_001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\athakur\Documents\MDOT\rstars\src\main\java\TestSuite\MDOT\Scenarios\MDOT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\athakur\Documents\MDOT\rstar\rstars\src\main\java\TestSuite\MDOT\Scenarios\MDOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4A6C5A-72DC-4768-8D45-46D3D9E3B60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3CE2A7-7EF9-4777-A8F2-932611E5B479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ED1DE3A2-7D10-4EDF-83CE-8D5FA019BAB9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>BusinessModule</t>
   </si>
@@ -96,12 +96,6 @@
     <t>Edit Profile</t>
   </si>
   <si>
-    <t>NextProfile</t>
-  </si>
-  <si>
-    <t>Next Profile</t>
-  </si>
-  <si>
     <t>TC_SM_FOU_DeleteProfile</t>
   </si>
   <si>
@@ -124,6 +118,30 @@
   </si>
   <si>
     <t>Logout</t>
+  </si>
+  <si>
+    <t>Nav_NextProfile_and_AddNewProfile</t>
+  </si>
+  <si>
+    <t>Open next profile</t>
+  </si>
+  <si>
+    <t>Adding New Profile Via Details Page</t>
+  </si>
+  <si>
+    <t>Recalling Existing Profile</t>
+  </si>
+  <si>
+    <t>Recall_Confirm</t>
+  </si>
+  <si>
+    <t>Confirm Alert Box</t>
+  </si>
+  <si>
+    <t>LastProcDateVerify</t>
+  </si>
+  <si>
+    <t>Verify Last Proc date</t>
   </si>
 </sst>
 </file>
@@ -520,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05B2E18-436A-488F-94B9-FF593DC035ED}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -581,10 +599,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
@@ -661,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
@@ -701,7 +719,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>19</v>
@@ -721,78 +739,158 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
+    <row r="17" spans="1:6" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>